<commit_message>
changed daq in bom
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -45,13 +45,7 @@
     <t>Data Acquisition Card</t>
   </si>
   <si>
-    <t>USB-6351</t>
-  </si>
-  <si>
     <t>National Instruments</t>
-  </si>
-  <si>
-    <t>16 AI (16-Bit, 1.25 MS/s), 2 AO (2.86 MS/s), 24 DIO USB Multifunction I/O Multifunction I/O Device</t>
   </si>
   <si>
     <t>Electronics</t>
@@ -720,6 +714,12 @@
   <si>
     <t>R-30W-0050</t>
   </si>
+  <si>
+    <t>USB-6002</t>
+  </si>
+  <si>
+    <t>Low-cost DAQ USB Device</t>
+  </si>
 </sst>
 </file>
 
@@ -1275,8 +1275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z1018"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G91" sqref="G91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1397,25 +1397,25 @@
       <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>11</v>
+      <c r="E4" s="12" t="s">
+        <v>233</v>
       </c>
       <c r="F4" s="17"/>
       <c r="G4" s="17">
-        <v>2380</v>
+        <v>555</v>
       </c>
       <c r="H4" s="4">
         <v>1</v>
       </c>
       <c r="I4" s="17">
         <f>G4*H4</f>
-        <v>2380</v>
+        <v>555</v>
       </c>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -1466,7 +1466,7 @@
     <row r="6" spans="1:26" ht="15" customHeight="1">
       <c r="A6" s="1"/>
       <c r="B6" s="26" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C6" s="27"/>
       <c r="D6" s="28"/>
@@ -1496,13 +1496,13 @@
     <row r="7" spans="1:26" ht="15" customHeight="1">
       <c r="A7" s="1"/>
       <c r="B7" s="27" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C7" s="27">
         <v>232</v>
       </c>
       <c r="D7" s="28" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E7" s="28"/>
       <c r="F7" s="29">
@@ -1540,13 +1540,13 @@
     <row r="8" spans="1:26" ht="15" customHeight="1">
       <c r="A8" s="1"/>
       <c r="B8" s="27" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C8" s="27" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D8" s="28" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E8" s="28"/>
       <c r="F8" s="29"/>
@@ -1581,13 +1581,13 @@
     <row r="9" spans="1:26" ht="15" customHeight="1">
       <c r="A9" s="1"/>
       <c r="B9" s="27" t="s">
+        <v>227</v>
+      </c>
+      <c r="C9" s="27" t="s">
         <v>229</v>
       </c>
-      <c r="C9" s="27" t="s">
-        <v>231</v>
-      </c>
       <c r="D9" s="28" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E9" s="28"/>
       <c r="F9" s="29"/>
@@ -1622,13 +1622,13 @@
     <row r="10" spans="1:26" ht="15" customHeight="1">
       <c r="A10" s="1"/>
       <c r="B10" s="27" t="s">
+        <v>228</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>231</v>
+      </c>
+      <c r="D10" s="28" t="s">
         <v>230</v>
-      </c>
-      <c r="C10" s="27" t="s">
-        <v>233</v>
-      </c>
-      <c r="D10" s="28" t="s">
-        <v>232</v>
       </c>
       <c r="E10" s="28"/>
       <c r="F10" s="29"/>
@@ -1663,12 +1663,12 @@
     <row r="11" spans="1:26" ht="15" customHeight="1">
       <c r="A11" s="1"/>
       <c r="B11" s="27" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C11" s="27"/>
       <c r="D11" s="28"/>
       <c r="E11" s="33" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F11" s="29"/>
       <c r="G11" s="29">
@@ -1702,13 +1702,13 @@
     <row r="12" spans="1:26" ht="15" customHeight="1">
       <c r="A12" s="1"/>
       <c r="B12" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="28" t="s">
         <v>17</v>
-      </c>
-      <c r="C12" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="28" t="s">
-        <v>19</v>
       </c>
       <c r="E12" s="28"/>
       <c r="F12" s="29"/>
@@ -1743,13 +1743,13 @@
     <row r="13" spans="1:26" ht="15" customHeight="1">
       <c r="A13" s="1"/>
       <c r="B13" s="27" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D13" s="28" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E13" s="28"/>
       <c r="F13" s="29"/>
@@ -1784,16 +1784,16 @@
     <row r="14" spans="1:26" ht="15" customHeight="1">
       <c r="A14" s="1"/>
       <c r="B14" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="28" t="s">
+      <c r="E14" s="28" t="s">
         <v>23</v>
-      </c>
-      <c r="D14" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="E14" s="28" t="s">
-        <v>25</v>
       </c>
       <c r="F14" s="29"/>
       <c r="G14" s="29">
@@ -1827,16 +1827,16 @@
     <row r="15" spans="1:26" ht="15" customHeight="1">
       <c r="A15" s="1"/>
       <c r="B15" s="27" t="s">
+        <v>203</v>
+      </c>
+      <c r="C15" s="28" t="s">
+        <v>204</v>
+      </c>
+      <c r="D15" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="28" t="s">
         <v>205</v>
-      </c>
-      <c r="C15" s="28" t="s">
-        <v>206</v>
-      </c>
-      <c r="D15" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15" s="28" t="s">
-        <v>207</v>
       </c>
       <c r="F15" s="29"/>
       <c r="G15" s="29">
@@ -1870,16 +1870,16 @@
     <row r="16" spans="1:26" ht="15" customHeight="1">
       <c r="A16" s="1"/>
       <c r="B16" s="14" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C16" s="27">
         <v>61300211121</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="F16" s="17"/>
       <c r="G16" s="17">
@@ -1913,16 +1913,16 @@
     <row r="17" spans="1:26" ht="15" customHeight="1">
       <c r="A17" s="1"/>
       <c r="B17" s="14" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C17" s="27">
         <v>61300311121</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="F17" s="17"/>
       <c r="G17" s="17">
@@ -1956,16 +1956,16 @@
     <row r="18" spans="1:26" ht="15" customHeight="1">
       <c r="A18" s="1"/>
       <c r="B18" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="C18" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="E18" s="13" t="s">
         <v>218</v>
-      </c>
-      <c r="C18" s="28" t="s">
-        <v>219</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>211</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>220</v>
       </c>
       <c r="F18" s="17"/>
       <c r="G18" s="17">
@@ -1999,16 +1999,16 @@
     <row r="19" spans="1:26" ht="15" customHeight="1">
       <c r="A19" s="1"/>
       <c r="B19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="E19" s="6" t="s">
         <v>27</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>29</v>
       </c>
       <c r="F19" s="17"/>
       <c r="G19" s="17">
@@ -2042,16 +2042,16 @@
     <row r="20" spans="1:26" ht="15" customHeight="1">
       <c r="A20" s="1"/>
       <c r="B20" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="7" t="s">
         <v>30</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>32</v>
       </c>
       <c r="F20" s="17"/>
       <c r="G20" s="17">
@@ -2085,16 +2085,16 @@
     <row r="21" spans="1:26" ht="15" customHeight="1">
       <c r="A21" s="1"/>
       <c r="B21" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="E21" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>36</v>
       </c>
       <c r="F21" s="17"/>
       <c r="G21" s="17">
@@ -2128,16 +2128,16 @@
     <row r="22" spans="1:26" ht="15" customHeight="1">
       <c r="A22" s="1"/>
       <c r="B22" s="23" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C22" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="E22" s="12" t="s">
         <v>195</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>196</v>
-      </c>
-      <c r="E22" s="12" t="s">
-        <v>197</v>
       </c>
       <c r="F22" s="17"/>
       <c r="G22" s="17">
@@ -2171,16 +2171,16 @@
     <row r="23" spans="1:26" ht="15" customHeight="1">
       <c r="A23" s="1"/>
       <c r="B23" s="23" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D23" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="E23" s="12" t="s">
         <v>196</v>
-      </c>
-      <c r="E23" s="12" t="s">
-        <v>198</v>
       </c>
       <c r="F23" s="17"/>
       <c r="G23" s="17">
@@ -2214,16 +2214,16 @@
     <row r="24" spans="1:26" ht="15" customHeight="1">
       <c r="A24" s="1"/>
       <c r="B24" s="23" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F24" s="17"/>
       <c r="G24" s="17">
@@ -2257,16 +2257,16 @@
     <row r="25" spans="1:26" ht="15" customHeight="1">
       <c r="A25" s="1"/>
       <c r="B25" s="23" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C25" s="24" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="F25" s="17"/>
       <c r="G25" s="17">
@@ -2300,16 +2300,16 @@
     <row r="26" spans="1:26" ht="15" customHeight="1">
       <c r="A26" s="1"/>
       <c r="B26" s="23" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E26" s="25" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F26" s="17"/>
       <c r="G26" s="17">
@@ -2343,16 +2343,16 @@
     <row r="27" spans="1:26" ht="15" customHeight="1">
       <c r="A27" s="1"/>
       <c r="B27" s="30" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C27" s="31" t="s">
+        <v>213</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E27" s="13" t="s">
         <v>215</v>
-      </c>
-      <c r="D27" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E27" s="13" t="s">
-        <v>217</v>
       </c>
       <c r="F27" s="17"/>
       <c r="G27" s="17">
@@ -2386,16 +2386,16 @@
     <row r="28" spans="1:26" ht="15" customHeight="1">
       <c r="A28" s="1"/>
       <c r="B28" s="22" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C28" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E28" s="6" t="s">
         <v>37</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>39</v>
       </c>
       <c r="F28" s="17"/>
       <c r="G28" s="17">
@@ -2429,16 +2429,16 @@
     <row r="29" spans="1:26" ht="15" customHeight="1">
       <c r="A29" s="1"/>
       <c r="B29" s="22" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C29" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E29" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>42</v>
       </c>
       <c r="F29" s="17"/>
       <c r="G29" s="17">
@@ -2472,16 +2472,16 @@
     <row r="30" spans="1:26" ht="15" customHeight="1">
       <c r="A30" s="1"/>
       <c r="B30" s="22" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F30" s="17"/>
       <c r="G30" s="17">
@@ -2515,16 +2515,16 @@
     <row r="31" spans="1:26" ht="15" customHeight="1">
       <c r="A31" s="1"/>
       <c r="B31" s="22" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C31" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E31" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>47</v>
       </c>
       <c r="F31" s="17"/>
       <c r="G31" s="17">
@@ -2558,16 +2558,16 @@
     <row r="32" spans="1:26" ht="15" customHeight="1">
       <c r="A32" s="1"/>
       <c r="B32" s="22" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F32" s="17"/>
       <c r="G32" s="17">
@@ -2601,16 +2601,16 @@
     <row r="33" spans="1:26" ht="15" customHeight="1">
       <c r="A33" s="1"/>
       <c r="B33" s="22" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F33" s="17"/>
       <c r="G33" s="17">
@@ -2644,16 +2644,16 @@
     <row r="34" spans="1:26" ht="15" customHeight="1">
       <c r="A34" s="1"/>
       <c r="B34" s="14" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D34" s="13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E34" s="13" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F34" s="17"/>
       <c r="G34" s="17">
@@ -2687,16 +2687,16 @@
     <row r="35" spans="1:26" ht="15" customHeight="1">
       <c r="A35" s="1"/>
       <c r="B35" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D35" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="E35" s="4" t="s">
         <v>53</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>55</v>
       </c>
       <c r="F35" s="17"/>
       <c r="G35" s="17">
@@ -2758,7 +2758,7 @@
     <row r="37" spans="1:26" ht="15" customHeight="1">
       <c r="A37" s="1"/>
       <c r="B37" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="4"/>
@@ -2788,16 +2788,16 @@
     <row r="38" spans="1:26" ht="15" customHeight="1">
       <c r="A38" s="1"/>
       <c r="B38" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D38" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C38" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>66</v>
-      </c>
       <c r="E38" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F38" s="17">
         <v>2500</v>
@@ -2834,16 +2834,16 @@
     <row r="39" spans="1:26" ht="15" customHeight="1">
       <c r="A39" s="1"/>
       <c r="B39" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E39" s="4" t="s">
         <v>67</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>69</v>
       </c>
       <c r="F39" s="17">
         <v>200</v>
@@ -2880,16 +2880,16 @@
     <row r="40" spans="1:26" ht="15" customHeight="1">
       <c r="A40" s="1"/>
       <c r="B40" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D40" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="E40" s="4" t="s">
         <v>71</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>73</v>
       </c>
       <c r="F40" s="17"/>
       <c r="G40" s="17">
@@ -2923,16 +2923,16 @@
     <row r="41" spans="1:26" ht="15" customHeight="1">
       <c r="A41" s="1"/>
       <c r="B41" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="C41" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="C41" s="14" t="s">
-        <v>137</v>
-      </c>
       <c r="D41" s="12" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E41" s="12" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F41" s="17"/>
       <c r="G41" s="17">
@@ -2966,16 +2966,16 @@
     <row r="42" spans="1:26" ht="15" customHeight="1">
       <c r="A42" s="1"/>
       <c r="B42" s="14" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D42" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="E42" s="12" t="s">
         <v>138</v>
-      </c>
-      <c r="E42" s="12" t="s">
-        <v>140</v>
       </c>
       <c r="F42" s="17"/>
       <c r="G42" s="17">
@@ -3009,16 +3009,16 @@
     <row r="43" spans="1:26" ht="15" customHeight="1">
       <c r="A43" s="1"/>
       <c r="B43" s="11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D43" s="13" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E43" s="13" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F43" s="17"/>
       <c r="G43" s="17">
@@ -3052,16 +3052,16 @@
     <row r="44" spans="1:26" ht="15" customHeight="1">
       <c r="A44" s="1"/>
       <c r="B44" s="11" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D44" s="13" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E44" s="13" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F44" s="17"/>
       <c r="G44" s="17">
@@ -3095,16 +3095,16 @@
     <row r="45" spans="1:26" ht="15" customHeight="1">
       <c r="A45" s="1"/>
       <c r="B45" s="11" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D45" s="13" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E45" s="13" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F45" s="17"/>
       <c r="G45" s="17">
@@ -3138,16 +3138,16 @@
     <row r="46" spans="1:26" ht="15" customHeight="1">
       <c r="A46" s="1"/>
       <c r="B46" s="14" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D46" s="13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F46" s="17"/>
       <c r="G46" s="17">
@@ -3181,16 +3181,16 @@
     <row r="47" spans="1:26" ht="15" customHeight="1">
       <c r="A47" s="1"/>
       <c r="B47" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C47" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E47" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="C47" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E47" s="4" t="s">
-        <v>58</v>
       </c>
       <c r="F47" s="17"/>
       <c r="G47" s="17">
@@ -3224,16 +3224,16 @@
     <row r="48" spans="1:26" ht="15" customHeight="1">
       <c r="A48" s="1"/>
       <c r="B48" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C48" s="2">
         <v>112420</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F48" s="17"/>
       <c r="G48" s="17">
@@ -3267,16 +3267,16 @@
     <row r="49" spans="1:26" ht="15" customHeight="1">
       <c r="A49" s="1"/>
       <c r="B49" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C49" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E49" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="C49" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E49" s="4" t="s">
-        <v>61</v>
       </c>
       <c r="F49" s="17"/>
       <c r="G49" s="17">
@@ -3310,16 +3310,16 @@
     <row r="50" spans="1:26" ht="15" customHeight="1">
       <c r="A50" s="1"/>
       <c r="B50" s="11" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C50" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D50" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F50" s="17"/>
       <c r="G50" s="19">
@@ -3353,16 +3353,16 @@
     <row r="51" spans="1:26" ht="15" customHeight="1">
       <c r="A51" s="1"/>
       <c r="B51" s="11" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C51" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="D51" s="13" t="s">
         <v>159</v>
       </c>
-      <c r="D51" s="13" t="s">
-        <v>161</v>
-      </c>
       <c r="E51" s="13" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F51" s="17"/>
       <c r="G51" s="17">
@@ -3396,16 +3396,16 @@
     <row r="52" spans="1:26" ht="15" customHeight="1">
       <c r="A52" s="1"/>
       <c r="B52" s="11" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C52" s="14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E52" s="13" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F52" s="17"/>
       <c r="G52" s="17">
@@ -3439,16 +3439,16 @@
     <row r="53" spans="1:26" ht="15" customHeight="1">
       <c r="A53" s="1"/>
       <c r="B53" s="11" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C53" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="D53" s="13" t="s">
         <v>169</v>
       </c>
-      <c r="D53" s="13" t="s">
-        <v>171</v>
-      </c>
       <c r="E53" s="13" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F53" s="17"/>
       <c r="G53" s="17">
@@ -3482,16 +3482,16 @@
     <row r="54" spans="1:26" ht="15" customHeight="1">
       <c r="A54" s="1"/>
       <c r="B54" s="11" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C54" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="D54" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="E54" s="13" t="s">
         <v>163</v>
-      </c>
-      <c r="D54" s="13" t="s">
-        <v>164</v>
-      </c>
-      <c r="E54" s="13" t="s">
-        <v>165</v>
       </c>
       <c r="F54" s="17"/>
       <c r="G54" s="17">
@@ -3525,16 +3525,16 @@
     <row r="55" spans="1:26" ht="15" customHeight="1">
       <c r="A55" s="1"/>
       <c r="B55" s="11" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C55" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="D55" s="13" t="s">
         <v>166</v>
       </c>
-      <c r="D55" s="13" t="s">
-        <v>168</v>
-      </c>
       <c r="E55" s="13" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F55" s="17"/>
       <c r="G55" s="17">
@@ -3596,7 +3596,7 @@
     <row r="57" spans="1:26" ht="15" customHeight="1">
       <c r="A57" s="1"/>
       <c r="B57" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" s="4"/>
@@ -3626,16 +3626,16 @@
     <row r="58" spans="1:26" ht="15" customHeight="1">
       <c r="A58" s="1"/>
       <c r="B58" s="14" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C58" s="14" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D58" s="13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E58" s="13" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F58" s="17"/>
       <c r="G58" s="17">
@@ -3669,16 +3669,16 @@
     <row r="59" spans="1:26" ht="15" customHeight="1">
       <c r="A59" s="1"/>
       <c r="B59" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="C59" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="D59" s="13" t="s">
         <v>190</v>
       </c>
-      <c r="C59" s="14" t="s">
+      <c r="E59" s="13" t="s">
         <v>191</v>
-      </c>
-      <c r="D59" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="E59" s="13" t="s">
-        <v>193</v>
       </c>
       <c r="F59" s="17">
         <v>9.49</v>
@@ -3715,16 +3715,16 @@
     <row r="60" spans="1:26" ht="15" customHeight="1">
       <c r="A60" s="1"/>
       <c r="B60" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C60" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="D60" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C60" s="14" t="s">
+      <c r="E60" s="4" t="s">
         <v>76</v>
-      </c>
-      <c r="D60" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="E60" s="4" t="s">
-        <v>78</v>
       </c>
       <c r="F60" s="17">
         <v>56.5</v>
@@ -3761,16 +3761,16 @@
     <row r="61" spans="1:26" ht="15" customHeight="1">
       <c r="A61" s="1"/>
       <c r="B61" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C61" s="11" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D61" s="12" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E61" s="12" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F61" s="17"/>
       <c r="G61" s="17">
@@ -3804,16 +3804,16 @@
     <row r="62" spans="1:26" ht="15" customHeight="1">
       <c r="A62" s="1"/>
       <c r="B62" s="14" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C62" s="14" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D62" s="13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E62" s="13" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F62" s="17"/>
       <c r="G62" s="17">
@@ -3847,16 +3847,16 @@
     <row r="63" spans="1:26" ht="15" customHeight="1">
       <c r="A63" s="1"/>
       <c r="B63" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="C63" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="D63" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="E63" s="13" t="s">
         <v>177</v>
-      </c>
-      <c r="C63" s="14" t="s">
-        <v>178</v>
-      </c>
-      <c r="D63" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="E63" s="13" t="s">
-        <v>179</v>
       </c>
       <c r="F63" s="17"/>
       <c r="G63" s="17">
@@ -3890,16 +3890,16 @@
     <row r="64" spans="1:26" ht="15" customHeight="1">
       <c r="A64" s="1"/>
       <c r="B64" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E64" s="4" t="s">
         <v>79</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D64" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="E64" s="4" t="s">
-        <v>81</v>
       </c>
       <c r="F64" s="17">
         <v>26.5</v>
@@ -3936,16 +3936,16 @@
     <row r="65" spans="1:26" ht="15" customHeight="1">
       <c r="A65" s="1"/>
       <c r="B65" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E65" s="7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F65" s="21">
         <v>14.25</v>
@@ -3982,16 +3982,16 @@
     <row r="66" spans="1:26" ht="15" customHeight="1">
       <c r="A66" s="1"/>
       <c r="B66" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E66" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F66" s="17">
         <v>12.59</v>
@@ -4028,16 +4028,16 @@
     <row r="67" spans="1:26" ht="15" customHeight="1">
       <c r="A67" s="1"/>
       <c r="B67" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C67" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E67" s="4" t="s">
         <v>86</v>
-      </c>
-      <c r="C67" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="D67" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="E67" s="4" t="s">
-        <v>88</v>
       </c>
       <c r="F67" s="17"/>
       <c r="G67" s="17">
@@ -4071,16 +4071,16 @@
     <row r="68" spans="1:26" ht="15" customHeight="1">
       <c r="A68" s="1"/>
       <c r="B68" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E68" s="9" t="s">
         <v>89</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D68" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="E68" s="9" t="s">
-        <v>91</v>
       </c>
       <c r="F68" s="17">
         <v>24.4</v>
@@ -4117,16 +4117,16 @@
     <row r="69" spans="1:26" ht="15" customHeight="1">
       <c r="A69" s="1"/>
       <c r="B69" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E69" s="4" t="s">
         <v>92</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D69" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="E69" s="4" t="s">
-        <v>94</v>
       </c>
       <c r="F69" s="17"/>
       <c r="G69" s="17">
@@ -4160,16 +4160,16 @@
     <row r="70" spans="1:26" ht="15" customHeight="1">
       <c r="A70" s="1"/>
       <c r="B70" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E70" s="4" t="s">
         <v>95</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="D70" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="E70" s="4" t="s">
-        <v>97</v>
       </c>
       <c r="F70" s="17">
         <v>59.25</v>
@@ -4206,16 +4206,16 @@
     <row r="71" spans="1:26" ht="15" customHeight="1">
       <c r="A71" s="1"/>
       <c r="B71" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E71" s="4" t="s">
         <v>98</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D71" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="E71" s="4" t="s">
-        <v>100</v>
       </c>
       <c r="F71" s="17">
         <v>20.2</v>
@@ -4252,16 +4252,16 @@
     <row r="72" spans="1:26" ht="15" customHeight="1">
       <c r="A72" s="1"/>
       <c r="B72" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E72" s="4" t="s">
         <v>101</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D72" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="E72" s="4" t="s">
-        <v>103</v>
       </c>
       <c r="F72" s="17">
         <v>51</v>
@@ -4298,16 +4298,16 @@
     <row r="73" spans="1:26" ht="15" customHeight="1">
       <c r="A73" s="1"/>
       <c r="B73" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D73" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E73" s="4" t="s">
         <v>104</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="D73" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="E73" s="4" t="s">
-        <v>106</v>
       </c>
       <c r="F73" s="17">
         <v>148</v>
@@ -4344,16 +4344,16 @@
     <row r="74" spans="1:26" ht="15" customHeight="1">
       <c r="A74" s="1"/>
       <c r="B74" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E74" s="7" t="s">
         <v>107</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="D74" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="E74" s="7" t="s">
-        <v>109</v>
       </c>
       <c r="F74" s="17">
         <v>75</v>
@@ -4390,16 +4390,16 @@
     <row r="75" spans="1:26" ht="15" customHeight="1">
       <c r="A75" s="1"/>
       <c r="B75" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C75" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="D75" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="E75" s="4" t="s">
         <v>110</v>
-      </c>
-      <c r="C75" s="14" t="s">
-        <v>189</v>
-      </c>
-      <c r="D75" s="13" t="s">
-        <v>188</v>
-      </c>
-      <c r="E75" s="4" t="s">
-        <v>112</v>
       </c>
       <c r="F75" s="17">
         <v>300</v>
@@ -4436,16 +4436,16 @@
     <row r="76" spans="1:26" ht="15" customHeight="1">
       <c r="A76" s="1"/>
       <c r="B76" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D76" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E76" s="4" t="s">
         <v>113</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D76" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="E76" s="4" t="s">
-        <v>115</v>
       </c>
       <c r="F76" s="17">
         <v>325</v>
@@ -4482,16 +4482,16 @@
     <row r="77" spans="1:26" ht="15" customHeight="1">
       <c r="A77" s="1"/>
       <c r="B77" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C77" s="14" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D77" s="13" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E77" s="12" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F77" s="17">
         <v>305</v>
@@ -4528,16 +4528,16 @@
     <row r="78" spans="1:26" ht="15" customHeight="1">
       <c r="A78" s="1"/>
       <c r="B78" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D78" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E78" s="4" t="s">
         <v>117</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="D78" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="E78" s="4" t="s">
-        <v>119</v>
       </c>
       <c r="F78" s="17">
         <v>6</v>
@@ -4574,16 +4574,16 @@
     <row r="79" spans="1:26" ht="15" customHeight="1">
       <c r="A79" s="1"/>
       <c r="B79" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D79" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E79" s="32" t="s">
         <v>120</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="D79" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="E79" s="32" t="s">
-        <v>122</v>
       </c>
       <c r="F79" s="17">
         <v>33.5</v>
@@ -4620,16 +4620,16 @@
     <row r="80" spans="1:26" ht="15" customHeight="1">
       <c r="A80" s="1"/>
       <c r="B80" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D80" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E80" s="4" t="s">
         <v>123</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="D80" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="E80" s="4" t="s">
-        <v>125</v>
       </c>
       <c r="F80" s="17">
         <v>132</v>
@@ -4666,16 +4666,16 @@
     <row r="81" spans="1:26" ht="15" customHeight="1">
       <c r="A81" s="1"/>
       <c r="B81" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C81" s="14" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E81" s="13" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F81" s="17"/>
       <c r="G81" s="17">
@@ -4743,11 +4743,11 @@
       <c r="F83" s="17"/>
       <c r="G83" s="20"/>
       <c r="H83" s="34" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="I83" s="18">
         <f>SUM($I$4)</f>
-        <v>2380</v>
+        <v>555</v>
       </c>
       <c r="J83" s="1"/>
       <c r="K83" s="1"/>
@@ -4776,7 +4776,7 @@
       <c r="F84" s="17"/>
       <c r="G84" s="20"/>
       <c r="H84" s="34" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="I84" s="18">
         <f>SUM($I$7:$I$35)</f>
@@ -4809,11 +4809,11 @@
       <c r="F85" s="17"/>
       <c r="G85" s="20"/>
       <c r="H85" s="34" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="I85" s="18">
-        <f>SUM($I38:$I$55)</f>
-        <v>3642.7500000000005</v>
+        <f>SUM($I58:$I$81)</f>
+        <v>2551.8589999999999</v>
       </c>
       <c r="J85" s="1"/>
       <c r="K85" s="1"/>
@@ -4842,11 +4842,11 @@
       <c r="F86" s="17"/>
       <c r="G86" s="20"/>
       <c r="H86" s="34" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="I86" s="18">
-        <f>SUM(I58:I81)</f>
-        <v>2551.8589999999999</v>
+        <f>SUM(I38:I55)</f>
+        <v>3642.7500000000005</v>
       </c>
       <c r="J86" s="1"/>
       <c r="K86" s="1"/>
@@ -4903,11 +4903,11 @@
       <c r="F88" s="17"/>
       <c r="G88" s="17"/>
       <c r="H88" s="35" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="I88" s="16">
-        <f>SUM(I85:I86)</f>
-        <v>6194.6090000000004</v>
+        <f>SUM(I83:I86)</f>
+        <v>6949.4017999999996</v>
       </c>
       <c r="J88" s="1"/>
       <c r="K88" s="1"/>

</xml_diff>

<commit_message>
reverted 6351 daq in bom
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -715,10 +715,10 @@
     <t>R-30W-0050</t>
   </si>
   <si>
-    <t>USB-6002</t>
+    <t>USB-6351</t>
   </si>
   <si>
-    <t>Low-cost DAQ USB Device</t>
+    <t>X Series Data Acquisition: 1.25MS/s 16 AI 24 DIO, 2 AO</t>
   </si>
 </sst>
 </file>
@@ -1275,8 +1275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z1018"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G91" sqref="G91"/>
+    <sheetView tabSelected="1" topLeftCell="C31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I93" sqref="I93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1408,14 +1408,14 @@
       </c>
       <c r="F4" s="17"/>
       <c r="G4" s="17">
-        <v>555</v>
+        <v>2385</v>
       </c>
       <c r="H4" s="4">
         <v>1</v>
       </c>
       <c r="I4" s="17">
         <f>G4*H4</f>
-        <v>555</v>
+        <v>2385</v>
       </c>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -4747,7 +4747,7 @@
       </c>
       <c r="I83" s="18">
         <f>SUM($I$4)</f>
-        <v>555</v>
+        <v>2385</v>
       </c>
       <c r="J83" s="1"/>
       <c r="K83" s="1"/>
@@ -4907,7 +4907,7 @@
       </c>
       <c r="I88" s="16">
         <f>SUM(I83:I86)</f>
-        <v>6949.4017999999996</v>
+        <v>8779.4017999999996</v>
       </c>
       <c r="J88" s="1"/>
       <c r="K88" s="1"/>

</xml_diff>

<commit_message>
thorlabs parts costs to usd
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="237">
   <si>
     <t>item</t>
   </si>
@@ -720,6 +720,15 @@
   <si>
     <t>X Series Data Acquisition: 1.25MS/s 16 AI 24 DIO, 2 AO</t>
   </si>
+  <si>
+    <t>Cost (USD)</t>
+  </si>
+  <si>
+    <t>CAD</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
 </sst>
 </file>
 
@@ -855,15 +864,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -871,7 +882,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -924,9 +935,6 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -972,6 +980,18 @@
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1275,8 +1295,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z1018"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I93" sqref="I93"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K85" sqref="K85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1286,10 +1306,11 @@
     <col min="3" max="3" width="21.28515625" customWidth="1"/>
     <col min="4" max="4" width="20.42578125" customWidth="1"/>
     <col min="5" max="5" width="46" customWidth="1"/>
-    <col min="6" max="7" width="12.28515625" style="19" customWidth="1"/>
+    <col min="6" max="7" width="12.28515625" style="18" customWidth="1"/>
     <col min="8" max="8" width="9.140625" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" style="19" customWidth="1"/>
-    <col min="10" max="26" width="8.7109375" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" style="18" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" customWidth="1"/>
+    <col min="11" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
@@ -1344,7 +1365,9 @@
         <v>6</v>
       </c>
       <c r="I2" s="17"/>
-      <c r="J2" s="1"/>
+      <c r="J2" s="35" t="s">
+        <v>234</v>
+      </c>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
@@ -1417,7 +1440,10 @@
         <f>G4*H4</f>
         <v>2385</v>
       </c>
-      <c r="J4" s="1"/>
+      <c r="J4" s="16">
+        <f>I4/1.3</f>
+        <v>1834.6153846153845</v>
+      </c>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -1445,7 +1471,10 @@
       <c r="G5" s="17"/>
       <c r="H5" s="4"/>
       <c r="I5" s="17"/>
-      <c r="J5" s="1"/>
+      <c r="J5" s="16">
+        <f t="shared" ref="J5:J68" si="0">I5/1.3</f>
+        <v>0</v>
+      </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
@@ -1465,17 +1494,20 @@
     </row>
     <row r="6" spans="1:26" ht="15" customHeight="1">
       <c r="A6" s="1"/>
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="27"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="29"/>
-      <c r="J6" s="1"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
@@ -1495,31 +1527,34 @@
     </row>
     <row r="7" spans="1:26" ht="15" customHeight="1">
       <c r="A7" s="1"/>
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="27">
+      <c r="C7" s="26">
         <v>232</v>
       </c>
-      <c r="D7" s="28" t="s">
+      <c r="D7" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="28"/>
-      <c r="F7" s="29">
+      <c r="E7" s="27"/>
+      <c r="F7" s="28">
         <v>0.6</v>
       </c>
-      <c r="G7" s="29">
+      <c r="G7" s="28">
         <f>F7*1.3</f>
         <v>0.78</v>
       </c>
-      <c r="H7" s="28">
+      <c r="H7" s="27">
         <v>4</v>
       </c>
-      <c r="I7" s="29">
+      <c r="I7" s="28">
         <f>G7*H7</f>
         <v>3.12</v>
       </c>
-      <c r="J7" s="1"/>
+      <c r="J7" s="16">
+        <f t="shared" si="0"/>
+        <v>2.4</v>
+      </c>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
@@ -1539,28 +1574,31 @@
     </row>
     <row r="8" spans="1:26" ht="15" customHeight="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="26" t="s">
         <v>171</v>
       </c>
-      <c r="D8" s="28" t="s">
+      <c r="D8" s="27" t="s">
         <v>222</v>
       </c>
-      <c r="E8" s="28"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29">
+      <c r="E8" s="27"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28">
         <v>4.4400000000000004</v>
       </c>
-      <c r="H8" s="28">
+      <c r="H8" s="27">
         <v>1</v>
       </c>
-      <c r="I8" s="29">
+      <c r="I8" s="28">
         <f>G8*H8</f>
         <v>4.4400000000000004</v>
       </c>
-      <c r="J8" s="1"/>
+      <c r="J8" s="16">
+        <f t="shared" si="0"/>
+        <v>3.4153846153846157</v>
+      </c>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
@@ -1580,28 +1618,31 @@
     </row>
     <row r="9" spans="1:26" ht="15" customHeight="1">
       <c r="A9" s="1"/>
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="26" t="s">
         <v>227</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="26" t="s">
         <v>229</v>
       </c>
-      <c r="D9" s="28" t="s">
+      <c r="D9" s="27" t="s">
         <v>230</v>
       </c>
-      <c r="E9" s="28"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="29">
+      <c r="E9" s="27"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28">
         <v>10.1</v>
       </c>
-      <c r="H9" s="28">
+      <c r="H9" s="27">
         <v>1</v>
       </c>
-      <c r="I9" s="29">
-        <f t="shared" ref="I9:I10" si="0">G9*H9</f>
+      <c r="I9" s="28">
+        <f t="shared" ref="I9:I10" si="1">G9*H9</f>
         <v>10.1</v>
       </c>
-      <c r="J9" s="1"/>
+      <c r="J9" s="16">
+        <f t="shared" si="0"/>
+        <v>7.7692307692307683</v>
+      </c>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
@@ -1621,28 +1662,31 @@
     </row>
     <row r="10" spans="1:26" ht="15" customHeight="1">
       <c r="A10" s="1"/>
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="26" t="s">
         <v>228</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="26" t="s">
         <v>231</v>
       </c>
-      <c r="D10" s="28" t="s">
+      <c r="D10" s="27" t="s">
         <v>230</v>
       </c>
-      <c r="E10" s="28"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29">
+      <c r="E10" s="27"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28">
         <v>10.1</v>
       </c>
-      <c r="H10" s="28">
+      <c r="H10" s="27">
         <v>1</v>
       </c>
-      <c r="I10" s="29">
+      <c r="I10" s="28">
+        <f t="shared" si="1"/>
+        <v>10.1</v>
+      </c>
+      <c r="J10" s="16">
         <f t="shared" si="0"/>
-        <v>10.1</v>
-      </c>
-      <c r="J10" s="1"/>
+        <v>7.7692307692307683</v>
+      </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
@@ -1662,26 +1706,29 @@
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1">
       <c r="A11" s="1"/>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="27"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="33" t="s">
+      <c r="C11" s="26"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="32" t="s">
         <v>223</v>
       </c>
-      <c r="F11" s="29"/>
-      <c r="G11" s="29">
+      <c r="F11" s="28"/>
+      <c r="G11" s="28">
         <v>60</v>
       </c>
-      <c r="H11" s="28">
+      <c r="H11" s="27">
         <v>1</v>
       </c>
-      <c r="I11" s="29">
-        <f t="shared" ref="I11:I35" si="1">G11*H11</f>
+      <c r="I11" s="28">
+        <f t="shared" ref="I11:I35" si="2">G11*H11</f>
         <v>60</v>
       </c>
-      <c r="J11" s="1"/>
+      <c r="J11" s="16">
+        <f t="shared" si="0"/>
+        <v>46.153846153846153</v>
+      </c>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
@@ -1701,28 +1748,31 @@
     </row>
     <row r="12" spans="1:26" ht="15" customHeight="1">
       <c r="A12" s="1"/>
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="28" t="s">
+      <c r="C12" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="28"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="29">
+      <c r="E12" s="27"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28">
         <v>0.66</v>
       </c>
-      <c r="H12" s="28">
+      <c r="H12" s="27">
         <v>1</v>
       </c>
-      <c r="I12" s="29">
-        <f t="shared" si="1"/>
+      <c r="I12" s="28">
+        <f t="shared" si="2"/>
         <v>0.66</v>
       </c>
-      <c r="J12" s="1"/>
+      <c r="J12" s="16">
+        <f t="shared" si="0"/>
+        <v>0.50769230769230766</v>
+      </c>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
@@ -1742,28 +1792,31 @@
     </row>
     <row r="13" spans="1:26" ht="15" customHeight="1">
       <c r="A13" s="1"/>
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="28" t="s">
+      <c r="C13" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="28" t="s">
+      <c r="D13" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="28"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29">
+      <c r="E13" s="27"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28">
         <v>0.64</v>
       </c>
-      <c r="H13" s="28">
+      <c r="H13" s="27">
         <v>1</v>
       </c>
-      <c r="I13" s="29">
-        <f t="shared" si="1"/>
+      <c r="I13" s="28">
+        <f t="shared" si="2"/>
         <v>0.64</v>
       </c>
-      <c r="J13" s="1"/>
+      <c r="J13" s="16">
+        <f t="shared" si="0"/>
+        <v>0.49230769230769228</v>
+      </c>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
@@ -1783,30 +1836,33 @@
     </row>
     <row r="14" spans="1:26" ht="15" customHeight="1">
       <c r="A14" s="1"/>
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="28" t="s">
+      <c r="C14" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="28" t="s">
+      <c r="D14" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="28" t="s">
+      <c r="E14" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="29"/>
-      <c r="G14" s="29">
+      <c r="F14" s="28"/>
+      <c r="G14" s="28">
         <v>12.84</v>
       </c>
-      <c r="H14" s="28">
+      <c r="H14" s="27">
         <v>1</v>
       </c>
-      <c r="I14" s="29">
-        <f t="shared" si="1"/>
+      <c r="I14" s="28">
+        <f t="shared" si="2"/>
         <v>12.84</v>
       </c>
-      <c r="J14" s="1"/>
+      <c r="J14" s="16">
+        <f t="shared" si="0"/>
+        <v>9.8769230769230774</v>
+      </c>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
@@ -1826,30 +1882,33 @@
     </row>
     <row r="15" spans="1:26" ht="15" customHeight="1">
       <c r="A15" s="1"/>
-      <c r="B15" s="27" t="s">
+      <c r="B15" s="26" t="s">
         <v>203</v>
       </c>
-      <c r="C15" s="28" t="s">
+      <c r="C15" s="27" t="s">
         <v>204</v>
       </c>
-      <c r="D15" s="28" t="s">
+      <c r="D15" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="28" t="s">
+      <c r="E15" s="27" t="s">
         <v>205</v>
       </c>
-      <c r="F15" s="29"/>
-      <c r="G15" s="29">
+      <c r="F15" s="28"/>
+      <c r="G15" s="28">
         <v>5.96</v>
       </c>
-      <c r="H15" s="28">
+      <c r="H15" s="27">
         <v>2</v>
       </c>
-      <c r="I15" s="29">
-        <f t="shared" si="1"/>
+      <c r="I15" s="28">
+        <f t="shared" si="2"/>
         <v>11.92</v>
       </c>
-      <c r="J15" s="1"/>
+      <c r="J15" s="16">
+        <f t="shared" si="0"/>
+        <v>9.1692307692307686</v>
+      </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
@@ -1872,7 +1931,7 @@
       <c r="B16" s="14" t="s">
         <v>211</v>
       </c>
-      <c r="C16" s="27">
+      <c r="C16" s="26">
         <v>61300211121</v>
       </c>
       <c r="D16" s="13" t="s">
@@ -1889,10 +1948,13 @@
         <v>20</v>
       </c>
       <c r="I16" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.6</v>
       </c>
-      <c r="J16" s="1"/>
+      <c r="J16" s="16">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
@@ -1915,7 +1977,7 @@
       <c r="B17" s="14" t="s">
         <v>210</v>
       </c>
-      <c r="C17" s="27">
+      <c r="C17" s="26">
         <v>61300311121</v>
       </c>
       <c r="D17" s="13" t="s">
@@ -1932,10 +1994,13 @@
         <v>20</v>
       </c>
       <c r="I17" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.6</v>
       </c>
-      <c r="J17" s="1"/>
+      <c r="J17" s="16">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
@@ -1958,7 +2023,7 @@
       <c r="B18" s="14" t="s">
         <v>216</v>
       </c>
-      <c r="C18" s="28" t="s">
+      <c r="C18" s="27" t="s">
         <v>217</v>
       </c>
       <c r="D18" s="13" t="s">
@@ -1975,10 +2040,13 @@
         <v>10</v>
       </c>
       <c r="I18" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.7</v>
       </c>
-      <c r="J18" s="1"/>
+      <c r="J18" s="16">
+        <f t="shared" si="0"/>
+        <v>2.8461538461538463</v>
+      </c>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
@@ -2018,10 +2086,13 @@
         <v>1</v>
       </c>
       <c r="I19" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.7</v>
       </c>
-      <c r="J19" s="1"/>
+      <c r="J19" s="16">
+        <f t="shared" si="0"/>
+        <v>1.3076923076923077</v>
+      </c>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
@@ -2061,10 +2132,13 @@
         <v>1</v>
       </c>
       <c r="I20" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.42</v>
       </c>
-      <c r="J20" s="1"/>
+      <c r="J20" s="16">
+        <f t="shared" si="0"/>
+        <v>6.476923076923077</v>
+      </c>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
@@ -2084,7 +2158,7 @@
     </row>
     <row r="21" spans="1:26" ht="15" customHeight="1">
       <c r="A21" s="1"/>
-      <c r="B21" s="22" t="s">
+      <c r="B21" s="21" t="s">
         <v>31</v>
       </c>
       <c r="C21" s="2" t="s">
@@ -2104,10 +2178,13 @@
         <v>4</v>
       </c>
       <c r="I21" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.24</v>
       </c>
-      <c r="J21" s="1"/>
+      <c r="J21" s="16">
+        <f t="shared" si="0"/>
+        <v>2.4923076923076923</v>
+      </c>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
@@ -2127,7 +2204,7 @@
     </row>
     <row r="22" spans="1:26" ht="15" customHeight="1">
       <c r="A22" s="1"/>
-      <c r="B22" s="23" t="s">
+      <c r="B22" s="22" t="s">
         <v>31</v>
       </c>
       <c r="C22" s="11" t="s">
@@ -2147,10 +2224,13 @@
         <v>20</v>
       </c>
       <c r="I22" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.98E-2</v>
       </c>
-      <c r="J22" s="1"/>
+      <c r="J22" s="16">
+        <f t="shared" si="0"/>
+        <v>2.2923076923076921E-2</v>
+      </c>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
@@ -2170,10 +2250,10 @@
     </row>
     <row r="23" spans="1:26" ht="15" customHeight="1">
       <c r="A23" s="1"/>
-      <c r="B23" s="23" t="s">
+      <c r="B23" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="24" t="s">
+      <c r="C23" s="23" t="s">
         <v>197</v>
       </c>
       <c r="D23" s="12" t="s">
@@ -2190,10 +2270,13 @@
         <v>20</v>
       </c>
       <c r="I23" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.8400000000000004E-2</v>
       </c>
-      <c r="J23" s="1"/>
+      <c r="J23" s="16">
+        <f t="shared" si="0"/>
+        <v>2.9538461538461541E-2</v>
+      </c>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
@@ -2213,10 +2296,10 @@
     </row>
     <row r="24" spans="1:26" ht="15" customHeight="1">
       <c r="A24" s="1"/>
-      <c r="B24" s="23" t="s">
+      <c r="B24" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="24" t="s">
+      <c r="C24" s="23" t="s">
         <v>198</v>
       </c>
       <c r="D24" s="12" t="s">
@@ -2233,10 +2316,13 @@
         <v>20</v>
       </c>
       <c r="I24" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.8400000000000004E-2</v>
       </c>
-      <c r="J24" s="1"/>
+      <c r="J24" s="16">
+        <f t="shared" si="0"/>
+        <v>2.9538461538461541E-2</v>
+      </c>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
@@ -2256,10 +2342,10 @@
     </row>
     <row r="25" spans="1:26" ht="15" customHeight="1">
       <c r="A25" s="1"/>
-      <c r="B25" s="23" t="s">
+      <c r="B25" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="24" t="s">
+      <c r="C25" s="23" t="s">
         <v>200</v>
       </c>
       <c r="D25" s="12" t="s">
@@ -2276,10 +2362,13 @@
         <v>20</v>
       </c>
       <c r="I25" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.8400000000000004E-2</v>
       </c>
-      <c r="J25" s="1"/>
+      <c r="J25" s="16">
+        <f t="shared" si="0"/>
+        <v>2.9538461538461541E-2</v>
+      </c>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
@@ -2299,7 +2388,7 @@
     </row>
     <row r="26" spans="1:26" ht="15" customHeight="1">
       <c r="A26" s="1"/>
-      <c r="B26" s="23" t="s">
+      <c r="B26" s="22" t="s">
         <v>31</v>
       </c>
       <c r="C26" s="14" t="s">
@@ -2308,7 +2397,7 @@
       <c r="D26" s="12" t="s">
         <v>194</v>
       </c>
-      <c r="E26" s="25" t="s">
+      <c r="E26" s="24" t="s">
         <v>202</v>
       </c>
       <c r="F26" s="17"/>
@@ -2319,10 +2408,13 @@
         <v>20</v>
       </c>
       <c r="I26" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.8400000000000004E-2</v>
       </c>
-      <c r="J26" s="1"/>
+      <c r="J26" s="16">
+        <f t="shared" si="0"/>
+        <v>2.9538461538461541E-2</v>
+      </c>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
@@ -2342,10 +2434,10 @@
     </row>
     <row r="27" spans="1:26" ht="15" customHeight="1">
       <c r="A27" s="1"/>
-      <c r="B27" s="30" t="s">
+      <c r="B27" s="29" t="s">
         <v>212</v>
       </c>
-      <c r="C27" s="31" t="s">
+      <c r="C27" s="30" t="s">
         <v>213</v>
       </c>
       <c r="D27" s="13" t="s">
@@ -2362,10 +2454,13 @@
         <v>10</v>
       </c>
       <c r="I27" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.9400000000000001E-2</v>
       </c>
-      <c r="J27" s="1"/>
+      <c r="J27" s="16">
+        <f t="shared" si="0"/>
+        <v>1.4923076923076923E-2</v>
+      </c>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
@@ -2385,7 +2480,7 @@
     </row>
     <row r="28" spans="1:26" ht="15" customHeight="1">
       <c r="A28" s="1"/>
-      <c r="B28" s="22" t="s">
+      <c r="B28" s="21" t="s">
         <v>31</v>
       </c>
       <c r="C28" s="2" t="s">
@@ -2405,10 +2500,13 @@
         <v>4</v>
       </c>
       <c r="I28" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.68</v>
       </c>
-      <c r="J28" s="1"/>
+      <c r="J28" s="16">
+        <f t="shared" si="0"/>
+        <v>4.3692307692307688</v>
+      </c>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
@@ -2428,7 +2526,7 @@
     </row>
     <row r="29" spans="1:26" ht="15" customHeight="1">
       <c r="A29" s="1"/>
-      <c r="B29" s="22" t="s">
+      <c r="B29" s="21" t="s">
         <v>31</v>
       </c>
       <c r="C29" s="2" t="s">
@@ -2448,10 +2546,13 @@
         <v>20</v>
       </c>
       <c r="I29" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.8</v>
       </c>
-      <c r="J29" s="1"/>
+      <c r="J29" s="16">
+        <f t="shared" si="0"/>
+        <v>2.9230769230769229</v>
+      </c>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
@@ -2471,7 +2572,7 @@
     </row>
     <row r="30" spans="1:26" ht="15" customHeight="1">
       <c r="A30" s="1"/>
-      <c r="B30" s="22" t="s">
+      <c r="B30" s="21" t="s">
         <v>31</v>
       </c>
       <c r="C30" s="2" t="s">
@@ -2491,10 +2592,13 @@
         <v>20</v>
       </c>
       <c r="I30" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.6</v>
       </c>
-      <c r="J30" s="1"/>
+      <c r="J30" s="16">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
@@ -2514,7 +2618,7 @@
     </row>
     <row r="31" spans="1:26" ht="15" customHeight="1">
       <c r="A31" s="1"/>
-      <c r="B31" s="22" t="s">
+      <c r="B31" s="21" t="s">
         <v>31</v>
       </c>
       <c r="C31" s="2" t="s">
@@ -2534,10 +2638,13 @@
         <v>20</v>
       </c>
       <c r="I31" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="J31" s="1"/>
+      <c r="J31" s="16">
+        <f t="shared" si="0"/>
+        <v>3.0769230769230766</v>
+      </c>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
@@ -2557,7 +2664,7 @@
     </row>
     <row r="32" spans="1:26" ht="15" customHeight="1">
       <c r="A32" s="1"/>
-      <c r="B32" s="22" t="s">
+      <c r="B32" s="21" t="s">
         <v>31</v>
       </c>
       <c r="C32" s="2" t="s">
@@ -2577,10 +2684,13 @@
         <v>20</v>
       </c>
       <c r="I32" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.4</v>
       </c>
-      <c r="J32" s="1"/>
+      <c r="J32" s="16">
+        <f t="shared" si="0"/>
+        <v>0.30769230769230771</v>
+      </c>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
@@ -2600,7 +2710,7 @@
     </row>
     <row r="33" spans="1:26" ht="15" customHeight="1">
       <c r="A33" s="1"/>
-      <c r="B33" s="22" t="s">
+      <c r="B33" s="21" t="s">
         <v>31</v>
       </c>
       <c r="C33" s="2" t="s">
@@ -2620,10 +2730,13 @@
         <v>20</v>
       </c>
       <c r="I33" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.2</v>
       </c>
-      <c r="J33" s="1"/>
+      <c r="J33" s="16">
+        <f t="shared" si="0"/>
+        <v>0.15384615384615385</v>
+      </c>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
@@ -2663,10 +2776,13 @@
         <v>3</v>
       </c>
       <c r="I34" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>37.83</v>
       </c>
-      <c r="J34" s="1"/>
+      <c r="J34" s="16">
+        <f t="shared" si="0"/>
+        <v>29.099999999999998</v>
+      </c>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
@@ -2706,10 +2822,13 @@
         <v>3</v>
       </c>
       <c r="I35" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="J35" s="1"/>
+      <c r="J35" s="16">
+        <f t="shared" si="0"/>
+        <v>6.9230769230769225</v>
+      </c>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
@@ -2737,7 +2856,10 @@
       <c r="G36" s="17"/>
       <c r="H36" s="4"/>
       <c r="I36" s="17"/>
-      <c r="J36" s="1"/>
+      <c r="J36" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
@@ -2767,7 +2889,10 @@
       <c r="G37" s="17"/>
       <c r="H37" s="4"/>
       <c r="I37" s="17"/>
-      <c r="J37" s="1"/>
+      <c r="J37" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
@@ -2803,7 +2928,7 @@
         <v>2500</v>
       </c>
       <c r="G38" s="17">
-        <f t="shared" ref="G38:G39" si="2">F38*1.3</f>
+        <f>F38*1.3</f>
         <v>3250</v>
       </c>
       <c r="H38" s="4">
@@ -2813,7 +2938,10 @@
         <f t="shared" ref="I38:I55" si="3">G38*H38</f>
         <v>3250</v>
       </c>
-      <c r="J38" s="1"/>
+      <c r="J38" s="16">
+        <f t="shared" si="0"/>
+        <v>2500</v>
+      </c>
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
@@ -2849,7 +2977,7 @@
         <v>200</v>
       </c>
       <c r="G39" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="G39" si="4">F39*1.3</f>
         <v>260</v>
       </c>
       <c r="H39" s="4">
@@ -2859,7 +2987,10 @@
         <f t="shared" si="3"/>
         <v>260</v>
       </c>
-      <c r="J39" s="1"/>
+      <c r="J39" s="16">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
@@ -2902,7 +3033,10 @@
         <f t="shared" si="3"/>
         <v>12.63</v>
       </c>
-      <c r="J40" s="1"/>
+      <c r="J40" s="16">
+        <f t="shared" si="0"/>
+        <v>9.7153846153846164</v>
+      </c>
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
       <c r="M40" s="1"/>
@@ -2945,7 +3079,10 @@
         <f t="shared" si="3"/>
         <v>10.68</v>
       </c>
-      <c r="J41" s="1"/>
+      <c r="J41" s="16">
+        <f t="shared" si="0"/>
+        <v>8.2153846153846146</v>
+      </c>
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
       <c r="M41" s="1"/>
@@ -2988,7 +3125,10 @@
         <f t="shared" si="3"/>
         <v>7.87</v>
       </c>
-      <c r="J42" s="1"/>
+      <c r="J42" s="16">
+        <f t="shared" si="0"/>
+        <v>6.0538461538461537</v>
+      </c>
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
@@ -3031,7 +3171,10 @@
         <f t="shared" si="3"/>
         <v>7.87</v>
       </c>
-      <c r="J43" s="1"/>
+      <c r="J43" s="16">
+        <f t="shared" si="0"/>
+        <v>6.0538461538461537</v>
+      </c>
       <c r="K43" s="1"/>
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
@@ -3074,7 +3217,10 @@
         <f t="shared" si="3"/>
         <v>4.28</v>
       </c>
-      <c r="J44" s="1"/>
+      <c r="J44" s="16">
+        <f t="shared" si="0"/>
+        <v>3.2923076923076926</v>
+      </c>
       <c r="K44" s="1"/>
       <c r="L44" s="1"/>
       <c r="M44" s="1"/>
@@ -3117,7 +3263,10 @@
         <f t="shared" si="3"/>
         <v>4.3499999999999996</v>
       </c>
-      <c r="J45" s="1"/>
+      <c r="J45" s="16">
+        <f t="shared" si="0"/>
+        <v>3.3461538461538458</v>
+      </c>
       <c r="K45" s="1"/>
       <c r="L45" s="1"/>
       <c r="M45" s="1"/>
@@ -3160,7 +3309,10 @@
         <f t="shared" si="3"/>
         <v>1.54</v>
       </c>
-      <c r="J46" s="1"/>
+      <c r="J46" s="16">
+        <f t="shared" si="0"/>
+        <v>1.1846153846153846</v>
+      </c>
       <c r="K46" s="1"/>
       <c r="L46" s="1"/>
       <c r="M46" s="1"/>
@@ -3200,10 +3352,13 @@
         <v>1</v>
       </c>
       <c r="I47" s="17">
-        <f t="shared" ref="I47" si="4">G47*H47</f>
+        <f t="shared" ref="I47" si="5">G47*H47</f>
         <v>14.3</v>
       </c>
-      <c r="J47" s="1"/>
+      <c r="J47" s="16">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
       <c r="K47" s="1"/>
       <c r="L47" s="1"/>
       <c r="M47" s="1"/>
@@ -3246,7 +3401,10 @@
         <f>G48*H48</f>
         <v>6</v>
       </c>
-      <c r="J48" s="1"/>
+      <c r="J48" s="16">
+        <f t="shared" si="0"/>
+        <v>4.615384615384615</v>
+      </c>
       <c r="K48" s="1"/>
       <c r="L48" s="1"/>
       <c r="M48" s="1"/>
@@ -3289,7 +3447,10 @@
         <f>G49*H49</f>
         <v>22</v>
       </c>
-      <c r="J49" s="1"/>
+      <c r="J49" s="16">
+        <f t="shared" si="0"/>
+        <v>16.923076923076923</v>
+      </c>
       <c r="K49" s="1"/>
       <c r="L49" s="1"/>
       <c r="M49" s="1"/>
@@ -3322,17 +3483,20 @@
         <v>148</v>
       </c>
       <c r="F50" s="17"/>
-      <c r="G50" s="19">
+      <c r="G50" s="18">
         <v>0.34</v>
       </c>
       <c r="H50" s="4">
         <v>1</v>
       </c>
       <c r="I50" s="17">
-        <f t="shared" ref="I50:I51" si="5">G50*H50</f>
+        <f t="shared" ref="I50:I51" si="6">G50*H50</f>
         <v>0.34</v>
       </c>
-      <c r="J50" s="1"/>
+      <c r="J50" s="16">
+        <f t="shared" si="0"/>
+        <v>0.26153846153846155</v>
+      </c>
       <c r="K50" s="1"/>
       <c r="L50" s="1"/>
       <c r="M50" s="1"/>
@@ -3372,10 +3536,13 @@
         <v>1</v>
       </c>
       <c r="I51" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>6.15</v>
       </c>
-      <c r="J51" s="1"/>
+      <c r="J51" s="16">
+        <f t="shared" si="0"/>
+        <v>4.7307692307692308</v>
+      </c>
       <c r="K51" s="1"/>
       <c r="L51" s="1"/>
       <c r="M51" s="1"/>
@@ -3418,7 +3585,10 @@
         <f t="shared" si="3"/>
         <v>7.75</v>
       </c>
-      <c r="J52" s="1"/>
+      <c r="J52" s="16">
+        <f t="shared" si="0"/>
+        <v>5.9615384615384617</v>
+      </c>
       <c r="K52" s="1"/>
       <c r="L52" s="1"/>
       <c r="M52" s="1"/>
@@ -3461,7 +3631,10 @@
         <f t="shared" si="3"/>
         <v>2.11</v>
       </c>
-      <c r="J53" s="1"/>
+      <c r="J53" s="16">
+        <f t="shared" si="0"/>
+        <v>1.6230769230769229</v>
+      </c>
       <c r="K53" s="1"/>
       <c r="L53" s="1"/>
       <c r="M53" s="1"/>
@@ -3504,7 +3677,10 @@
         <f t="shared" si="3"/>
         <v>15.53</v>
       </c>
-      <c r="J54" s="1"/>
+      <c r="J54" s="16">
+        <f t="shared" si="0"/>
+        <v>11.946153846153845</v>
+      </c>
       <c r="K54" s="1"/>
       <c r="L54" s="1"/>
       <c r="M54" s="1"/>
@@ -3547,7 +3723,10 @@
         <f t="shared" si="3"/>
         <v>9.35</v>
       </c>
-      <c r="J55" s="1"/>
+      <c r="J55" s="16">
+        <f t="shared" si="0"/>
+        <v>7.1923076923076916</v>
+      </c>
       <c r="K55" s="1"/>
       <c r="L55" s="1"/>
       <c r="M55" s="1"/>
@@ -3575,7 +3754,10 @@
       <c r="G56" s="17"/>
       <c r="H56" s="4"/>
       <c r="I56" s="17"/>
-      <c r="J56" s="1"/>
+      <c r="J56" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="K56" s="1"/>
       <c r="L56" s="1"/>
       <c r="M56" s="1"/>
@@ -3605,7 +3787,10 @@
       <c r="G57" s="17"/>
       <c r="H57" s="4"/>
       <c r="I57" s="17"/>
-      <c r="J57" s="1"/>
+      <c r="J57" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="K57" s="1"/>
       <c r="L57" s="1"/>
       <c r="M57" s="1"/>
@@ -3637,18 +3822,24 @@
       <c r="E58" s="13" t="s">
         <v>182</v>
       </c>
-      <c r="F58" s="17"/>
+      <c r="F58" s="17">
+        <v>48.5</v>
+      </c>
       <c r="G58" s="17">
-        <v>48.5</v>
+        <f t="shared" ref="G58:G80" si="7">F58*1.3</f>
+        <v>63.050000000000004</v>
       </c>
       <c r="H58" s="4">
         <v>1</v>
       </c>
       <c r="I58" s="17">
-        <f t="shared" ref="I58:I81" si="6">G58*H58</f>
+        <f t="shared" ref="I58:I81" si="8">G58*H58</f>
+        <v>63.050000000000004</v>
+      </c>
+      <c r="J58" s="16">
+        <f t="shared" si="0"/>
         <v>48.5</v>
       </c>
-      <c r="J58" s="1"/>
       <c r="K58" s="1"/>
       <c r="L58" s="1"/>
       <c r="M58" s="1"/>
@@ -3684,17 +3875,20 @@
         <v>9.49</v>
       </c>
       <c r="G59" s="17">
-        <f t="shared" ref="G59:G80" si="7">F59*1.3</f>
+        <f t="shared" si="7"/>
         <v>12.337000000000002</v>
       </c>
       <c r="H59" s="4">
         <v>1</v>
       </c>
       <c r="I59" s="17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>12.337000000000002</v>
       </c>
-      <c r="J59" s="1"/>
+      <c r="J59" s="16">
+        <f t="shared" si="0"/>
+        <v>9.49</v>
+      </c>
       <c r="K59" s="1"/>
       <c r="L59" s="1"/>
       <c r="M59" s="1"/>
@@ -3737,10 +3931,13 @@
         <v>1</v>
       </c>
       <c r="I60" s="17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>73.45</v>
       </c>
-      <c r="J60" s="1"/>
+      <c r="J60" s="16">
+        <f t="shared" si="0"/>
+        <v>56.5</v>
+      </c>
       <c r="K60" s="1"/>
       <c r="L60" s="1"/>
       <c r="M60" s="1"/>
@@ -3772,18 +3969,24 @@
       <c r="E61" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="F61" s="17"/>
+      <c r="F61" s="17">
+        <v>144</v>
+      </c>
       <c r="G61" s="17">
-        <v>144</v>
+        <f t="shared" si="7"/>
+        <v>187.20000000000002</v>
       </c>
       <c r="H61" s="4">
         <v>1</v>
       </c>
       <c r="I61" s="17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
+        <v>187.20000000000002</v>
+      </c>
+      <c r="J61" s="16">
+        <f t="shared" si="0"/>
         <v>144</v>
       </c>
-      <c r="J61" s="1"/>
       <c r="K61" s="1"/>
       <c r="L61" s="1"/>
       <c r="M61" s="1"/>
@@ -3815,18 +4018,24 @@
       <c r="E62" s="13" t="s">
         <v>178</v>
       </c>
-      <c r="F62" s="17"/>
+      <c r="F62" s="17">
+        <v>19.899999999999999</v>
+      </c>
       <c r="G62" s="17">
-        <v>19.899999999999999</v>
+        <f t="shared" si="7"/>
+        <v>25.869999999999997</v>
       </c>
       <c r="H62" s="4">
         <v>1</v>
       </c>
       <c r="I62" s="17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
+        <v>25.869999999999997</v>
+      </c>
+      <c r="J62" s="16">
+        <f t="shared" si="0"/>
         <v>19.899999999999999</v>
       </c>
-      <c r="J62" s="1"/>
       <c r="K62" s="1"/>
       <c r="L62" s="1"/>
       <c r="M62" s="1"/>
@@ -3858,18 +4067,24 @@
       <c r="E63" s="13" t="s">
         <v>177</v>
       </c>
-      <c r="F63" s="17"/>
+      <c r="F63" s="17">
+        <v>25.5</v>
+      </c>
       <c r="G63" s="17">
-        <v>25.5</v>
+        <f t="shared" si="7"/>
+        <v>33.15</v>
       </c>
       <c r="H63" s="4">
         <v>1</v>
       </c>
       <c r="I63" s="17">
-        <f t="shared" si="6"/>
-        <v>25.5</v>
-      </c>
-      <c r="J63" s="1"/>
+        <f t="shared" si="8"/>
+        <v>33.15</v>
+      </c>
+      <c r="J63" s="16">
+        <f t="shared" si="0"/>
+        <v>25.499999999999996</v>
+      </c>
       <c r="K63" s="1"/>
       <c r="L63" s="1"/>
       <c r="M63" s="1"/>
@@ -3912,10 +4127,13 @@
         <v>2</v>
       </c>
       <c r="I64" s="17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>68.900000000000006</v>
       </c>
-      <c r="J64" s="1"/>
+      <c r="J64" s="16">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
       <c r="K64" s="1"/>
       <c r="L64" s="1"/>
       <c r="M64" s="1"/>
@@ -3947,7 +4165,7 @@
       <c r="E65" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="F65" s="21">
+      <c r="F65" s="20">
         <v>14.25</v>
       </c>
       <c r="G65" s="17">
@@ -3958,10 +4176,13 @@
         <v>4</v>
       </c>
       <c r="I65" s="17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>74.100000000000009</v>
       </c>
-      <c r="J65" s="1"/>
+      <c r="J65" s="16">
+        <f t="shared" si="0"/>
+        <v>57.000000000000007</v>
+      </c>
       <c r="K65" s="1"/>
       <c r="L65" s="1"/>
       <c r="M65" s="1"/>
@@ -4004,10 +4225,13 @@
         <v>1</v>
       </c>
       <c r="I66" s="17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>16.367000000000001</v>
       </c>
-      <c r="J66" s="1"/>
+      <c r="J66" s="16">
+        <f t="shared" si="0"/>
+        <v>12.59</v>
+      </c>
       <c r="K66" s="1"/>
       <c r="L66" s="1"/>
       <c r="M66" s="1"/>
@@ -4039,18 +4263,24 @@
       <c r="E67" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="F67" s="17"/>
+      <c r="F67" s="17">
+        <v>18.399999999999999</v>
+      </c>
       <c r="G67" s="17">
-        <v>18.399999999999999</v>
+        <f t="shared" si="7"/>
+        <v>23.919999999999998</v>
       </c>
       <c r="H67" s="4">
         <v>1</v>
       </c>
       <c r="I67" s="17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
+        <v>23.919999999999998</v>
+      </c>
+      <c r="J67" s="16">
+        <f t="shared" si="0"/>
         <v>18.399999999999999</v>
       </c>
-      <c r="J67" s="1"/>
       <c r="K67" s="1"/>
       <c r="L67" s="1"/>
       <c r="M67" s="1"/>
@@ -4093,10 +4323,13 @@
         <v>1</v>
       </c>
       <c r="I68" s="17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>31.72</v>
       </c>
-      <c r="J68" s="1"/>
+      <c r="J68" s="16">
+        <f t="shared" si="0"/>
+        <v>24.4</v>
+      </c>
       <c r="K68" s="1"/>
       <c r="L68" s="1"/>
       <c r="M68" s="1"/>
@@ -4128,18 +4361,24 @@
       <c r="E69" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="F69" s="17"/>
+      <c r="F69" s="17">
+        <v>57.25</v>
+      </c>
       <c r="G69" s="17">
-        <v>57.25</v>
+        <f t="shared" si="7"/>
+        <v>74.424999999999997</v>
       </c>
       <c r="H69" s="4">
         <v>1</v>
       </c>
       <c r="I69" s="17">
-        <f t="shared" si="6"/>
-        <v>57.25</v>
-      </c>
-      <c r="J69" s="1"/>
+        <f t="shared" si="8"/>
+        <v>74.424999999999997</v>
+      </c>
+      <c r="J69" s="16">
+        <f t="shared" ref="J69:J86" si="9">I69/1.3</f>
+        <v>57.249999999999993</v>
+      </c>
       <c r="K69" s="1"/>
       <c r="L69" s="1"/>
       <c r="M69" s="1"/>
@@ -4182,10 +4421,13 @@
         <v>1</v>
       </c>
       <c r="I70" s="17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>77.025000000000006</v>
       </c>
-      <c r="J70" s="1"/>
+      <c r="J70" s="16">
+        <f t="shared" si="9"/>
+        <v>59.25</v>
+      </c>
       <c r="K70" s="1"/>
       <c r="L70" s="1"/>
       <c r="M70" s="1"/>
@@ -4228,10 +4470,13 @@
         <v>1</v>
       </c>
       <c r="I71" s="17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>26.26</v>
       </c>
-      <c r="J71" s="1"/>
+      <c r="J71" s="16">
+        <f t="shared" si="9"/>
+        <v>20.2</v>
+      </c>
       <c r="K71" s="1"/>
       <c r="L71" s="1"/>
       <c r="M71" s="1"/>
@@ -4274,10 +4519,13 @@
         <v>1</v>
       </c>
       <c r="I72" s="17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>66.3</v>
       </c>
-      <c r="J72" s="1"/>
+      <c r="J72" s="16">
+        <f t="shared" si="9"/>
+        <v>50.999999999999993</v>
+      </c>
       <c r="K72" s="1"/>
       <c r="L72" s="1"/>
       <c r="M72" s="1"/>
@@ -4320,10 +4568,13 @@
         <v>1</v>
       </c>
       <c r="I73" s="17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>192.4</v>
       </c>
-      <c r="J73" s="1"/>
+      <c r="J73" s="16">
+        <f t="shared" si="9"/>
+        <v>148</v>
+      </c>
       <c r="K73" s="1"/>
       <c r="L73" s="1"/>
       <c r="M73" s="1"/>
@@ -4366,10 +4617,13 @@
         <v>1</v>
       </c>
       <c r="I74" s="17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>97.5</v>
       </c>
-      <c r="J74" s="1"/>
+      <c r="J74" s="16">
+        <f t="shared" si="9"/>
+        <v>75</v>
+      </c>
       <c r="K74" s="1"/>
       <c r="L74" s="1"/>
       <c r="M74" s="1"/>
@@ -4412,10 +4666,13 @@
         <v>1</v>
       </c>
       <c r="I75" s="17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>390</v>
       </c>
-      <c r="J75" s="1"/>
+      <c r="J75" s="16">
+        <f t="shared" si="9"/>
+        <v>300</v>
+      </c>
       <c r="K75" s="1"/>
       <c r="L75" s="1"/>
       <c r="M75" s="1"/>
@@ -4458,10 +4715,13 @@
         <v>1</v>
       </c>
       <c r="I76" s="17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>422.5</v>
       </c>
-      <c r="J76" s="1"/>
+      <c r="J76" s="16">
+        <f t="shared" si="9"/>
+        <v>325</v>
+      </c>
       <c r="K76" s="1"/>
       <c r="L76" s="1"/>
       <c r="M76" s="1"/>
@@ -4504,10 +4764,13 @@
         <v>1</v>
       </c>
       <c r="I77" s="17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>396.5</v>
       </c>
-      <c r="J77" s="1"/>
+      <c r="J77" s="16">
+        <f t="shared" si="9"/>
+        <v>305</v>
+      </c>
       <c r="K77" s="1"/>
       <c r="L77" s="1"/>
       <c r="M77" s="1"/>
@@ -4550,10 +4813,13 @@
         <v>1</v>
       </c>
       <c r="I78" s="17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>7.8000000000000007</v>
       </c>
-      <c r="J78" s="1"/>
+      <c r="J78" s="16">
+        <f t="shared" si="9"/>
+        <v>6</v>
+      </c>
       <c r="K78" s="1"/>
       <c r="L78" s="1"/>
       <c r="M78" s="1"/>
@@ -4582,7 +4848,7 @@
       <c r="D79" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="E79" s="32" t="s">
+      <c r="E79" s="31" t="s">
         <v>120</v>
       </c>
       <c r="F79" s="17">
@@ -4596,10 +4862,13 @@
         <v>1</v>
       </c>
       <c r="I79" s="17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>43.550000000000004</v>
       </c>
-      <c r="J79" s="1"/>
+      <c r="J79" s="16">
+        <f t="shared" si="9"/>
+        <v>33.5</v>
+      </c>
       <c r="K79" s="1"/>
       <c r="L79" s="1"/>
       <c r="M79" s="1"/>
@@ -4642,10 +4911,13 @@
         <v>1</v>
       </c>
       <c r="I80" s="17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>171.6</v>
       </c>
-      <c r="J80" s="1"/>
+      <c r="J80" s="16">
+        <f t="shared" si="9"/>
+        <v>132</v>
+      </c>
       <c r="K80" s="1"/>
       <c r="L80" s="1"/>
       <c r="M80" s="1"/>
@@ -4685,10 +4957,13 @@
         <v>1</v>
       </c>
       <c r="I81" s="17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>70</v>
       </c>
-      <c r="J81" s="1"/>
+      <c r="J81" s="16">
+        <f t="shared" si="9"/>
+        <v>53.846153846153847</v>
+      </c>
       <c r="K81" s="1"/>
       <c r="L81" s="1"/>
       <c r="M81" s="1"/>
@@ -4716,7 +4991,7 @@
       <c r="G82" s="17"/>
       <c r="H82" s="10"/>
       <c r="I82" s="17"/>
-      <c r="J82" s="1"/>
+      <c r="J82" s="16"/>
       <c r="K82" s="1"/>
       <c r="L82" s="1"/>
       <c r="M82" s="1"/>
@@ -4741,15 +5016,18 @@
       <c r="D83" s="4"/>
       <c r="E83" s="4"/>
       <c r="F83" s="17"/>
-      <c r="G83" s="20"/>
-      <c r="H83" s="34" t="s">
+      <c r="G83" s="19"/>
+      <c r="H83" s="33" t="s">
         <v>128</v>
       </c>
-      <c r="I83" s="18">
+      <c r="I83" s="36">
         <f>SUM($I$4)</f>
         <v>2385</v>
       </c>
-      <c r="J83" s="1"/>
+      <c r="J83" s="37">
+        <f t="shared" si="9"/>
+        <v>1834.6153846153845</v>
+      </c>
       <c r="K83" s="1"/>
       <c r="L83" s="1"/>
       <c r="M83" s="1"/>
@@ -4774,15 +5052,18 @@
       <c r="D84" s="4"/>
       <c r="E84" s="4"/>
       <c r="F84" s="17"/>
-      <c r="G84" s="20"/>
-      <c r="H84" s="34" t="s">
+      <c r="G84" s="19"/>
+      <c r="H84" s="33" t="s">
         <v>127</v>
       </c>
-      <c r="I84" s="18">
+      <c r="I84" s="36">
         <f>SUM($I$7:$I$35)</f>
         <v>199.79279999999994</v>
       </c>
-      <c r="J84" s="1"/>
+      <c r="J84" s="37">
+        <f t="shared" si="9"/>
+        <v>153.68676923076919</v>
+      </c>
       <c r="K84" s="1"/>
       <c r="L84" s="1"/>
       <c r="M84" s="1"/>
@@ -4807,15 +5088,18 @@
       <c r="D85" s="4"/>
       <c r="E85" s="4"/>
       <c r="F85" s="17"/>
-      <c r="G85" s="20"/>
-      <c r="H85" s="34" t="s">
+      <c r="G85" s="19"/>
+      <c r="H85" s="33" t="s">
         <v>126</v>
       </c>
-      <c r="I85" s="18">
+      <c r="I85" s="36">
         <f>SUM($I58:$I$81)</f>
-        <v>2551.8589999999999</v>
-      </c>
-      <c r="J85" s="1"/>
+        <v>2645.9240000000004</v>
+      </c>
+      <c r="J85" s="37">
+        <f>I85/1.3</f>
+        <v>2035.3261538461541</v>
+      </c>
       <c r="K85" s="1"/>
       <c r="L85" s="1"/>
       <c r="M85" s="1"/>
@@ -4840,15 +5124,18 @@
       <c r="D86" s="4"/>
       <c r="E86" s="4"/>
       <c r="F86" s="17"/>
-      <c r="G86" s="20"/>
-      <c r="H86" s="34" t="s">
+      <c r="G86" s="19"/>
+      <c r="H86" s="33" t="s">
         <v>129</v>
       </c>
-      <c r="I86" s="18">
+      <c r="I86" s="36">
         <f>SUM(I38:I55)</f>
         <v>3642.7500000000005</v>
       </c>
-      <c r="J86" s="1"/>
+      <c r="J86" s="37">
+        <f t="shared" si="9"/>
+        <v>2802.1153846153848</v>
+      </c>
       <c r="K86" s="1"/>
       <c r="L86" s="1"/>
       <c r="M86" s="1"/>
@@ -4902,14 +5189,17 @@
       <c r="E88" s="4"/>
       <c r="F88" s="17"/>
       <c r="G88" s="17"/>
-      <c r="H88" s="35" t="s">
+      <c r="H88" s="34" t="s">
         <v>224</v>
       </c>
       <c r="I88" s="16">
         <f>SUM(I83:I86)</f>
-        <v>8779.4017999999996</v>
-      </c>
-      <c r="J88" s="1"/>
+        <v>8873.4668000000001</v>
+      </c>
+      <c r="J88" s="16">
+        <f>SUM(J83:J86)</f>
+        <v>6825.743692307693</v>
+      </c>
       <c r="K88" s="1"/>
       <c r="L88" s="1"/>
       <c r="M88" s="1"/>
@@ -4936,8 +5226,12 @@
       <c r="F89" s="17"/>
       <c r="G89" s="17"/>
       <c r="H89" s="1"/>
-      <c r="I89" s="16"/>
-      <c r="J89" s="1"/>
+      <c r="I89" s="38" t="s">
+        <v>235</v>
+      </c>
+      <c r="J89" s="34" t="s">
+        <v>236</v>
+      </c>
       <c r="K89" s="1"/>
       <c r="L89" s="1"/>
       <c r="M89" s="1"/>

</xml_diff>